<commit_message>
working on payment list
</commit_message>
<xml_diff>
--- a/databaseDetail.xlsx
+++ b/databaseDetail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\arvind\projects\alpha_backend_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24104AA8-B648-4B7B-8F3C-04C459EFDD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53107DA7-25B3-4FC8-ACC2-C8EAC7869D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7DA0EA3A-345D-4D7C-A864-207FCBB0D6AE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
   <si>
     <t>name</t>
   </si>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15215A8-07C0-4B1C-AD06-0D16F302D9A0}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,6 +777,9 @@
       <c r="F15" t="s">
         <v>16</v>
       </c>
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
@@ -799,6 +802,9 @@
       <c r="G19" t="s">
         <v>26</v>
       </c>
+      <c r="H19" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
@@ -821,6 +827,9 @@
       <c r="G22" t="s">
         <v>76</v>
       </c>
+      <c r="H22" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G23" t="s">
@@ -846,6 +855,9 @@
       <c r="G24" t="s">
         <v>75</v>
       </c>
+      <c r="H24" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
@@ -894,17 +906,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>45</v>
       </c>
@@ -923,13 +935,16 @@
       <c r="H36" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>50</v>
       </c>
@@ -940,12 +955,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
         <v>53</v>
       </c>
@@ -964,13 +979,16 @@
       <c r="H44" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
         <v>70</v>
       </c>
@@ -983,13 +1001,16 @@
       <c r="F49" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
         <v>72</v>
       </c>
@@ -1004,6 +1025,9 @@
       </c>
       <c r="G53" t="s">
         <v>61</v>
+      </c>
+      <c r="H53" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>